<commit_message>
Added the excel file with the false->true and true->false
</commit_message>
<xml_diff>
--- a/key_rules5.xlsx
+++ b/key_rules5.xlsx
@@ -1,23 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://entuedu-my.sharepoint.com/personal/ytan216_e_ntu_edu_sg/Documents/Desktop/BC2407/BC2407/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://entuedu-my.sharepoint.com/personal/syap020_e_ntu_edu_sg/Documents/NTU/Y2S2/BC2407 Analytics 2/Project/BC2407 project code/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="8_{9B37A76F-0E39-4CF9-A9F0-A8EBE120A321}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="23260" windowHeight="16940" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="key_rules5 (2)" sheetId="3" r:id="rId1"/>
     <sheet name="key_rules5" sheetId="1" r:id="rId2"/>
     <sheet name="final 11 rules" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -96,7 +108,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -965,24 +977,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="8" width="12" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="5.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1011,7 +1023,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1040,7 +1052,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1069,7 +1081,7 @@
         <v>3864</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1098,7 +1110,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1127,7 +1139,7 @@
         <v>3978</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1156,7 +1168,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -1185,7 +1197,7 @@
         <v>2616</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -1214,7 +1226,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -1243,7 +1255,7 @@
         <v>2742</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -1272,7 +1284,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1301,7 +1313,7 @@
         <v>3510</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1330,7 +1342,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1359,7 +1371,7 @@
         <v>3402</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -1388,7 +1400,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -1417,7 +1429,7 @@
         <v>3738</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -1446,7 +1458,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>11</v>
       </c>
@@ -1475,7 +1487,7 @@
         <v>3852</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -1504,7 +1516,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>11</v>
       </c>
@@ -1533,7 +1545,7 @@
         <v>3978</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -1562,7 +1574,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -1591,7 +1603,7 @@
         <v>2508</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>10</v>
       </c>
@@ -1620,7 +1632,7 @@
         <v>870</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>10</v>
       </c>
@@ -1649,7 +1661,7 @@
         <v>2844</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>10</v>
       </c>
@@ -1678,7 +1690,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>10</v>
       </c>
@@ -1707,7 +1719,7 @@
         <v>3390</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -1736,7 +1748,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>10</v>
       </c>
@@ -1765,7 +1777,7 @@
         <v>3288</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>10</v>
       </c>
@@ -1794,7 +1806,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>10</v>
       </c>
@@ -1823,7 +1835,7 @@
         <v>3738</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>10</v>
       </c>
@@ -1852,7 +1864,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>10</v>
       </c>
@@ -1881,7 +1893,7 @@
         <v>3636</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>10</v>
       </c>
@@ -1910,7 +1922,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>10</v>
       </c>
@@ -1939,7 +1951,7 @@
         <v>3864</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>17</v>
       </c>
@@ -1968,7 +1980,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>17</v>
       </c>
@@ -1997,7 +2009,7 @@
         <v>2952</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>17</v>
       </c>
@@ -2026,7 +2038,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>17</v>
       </c>
@@ -2055,7 +2067,7 @@
         <v>3408</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>19</v>
       </c>
@@ -2084,7 +2096,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>19</v>
       </c>
@@ -2113,7 +2125,7 @@
         <v>2742</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>19</v>
       </c>
@@ -2142,7 +2154,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>19</v>
       </c>
@@ -2171,7 +2183,7 @@
         <v>3420</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>16</v>
       </c>
@@ -2200,7 +2212,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>16</v>
       </c>
@@ -2229,7 +2241,7 @@
         <v>2724</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>16</v>
       </c>
@@ -2258,7 +2270,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>16</v>
       </c>
@@ -2287,7 +2299,7 @@
         <v>2748</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>16</v>
       </c>
@@ -2316,7 +2328,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>16</v>
       </c>
@@ -2345,7 +2357,7 @@
         <v>3738</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>16</v>
       </c>
@@ -2374,7 +2386,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>16</v>
       </c>
@@ -2403,7 +2415,7 @@
         <v>3504</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>16</v>
       </c>
@@ -2432,7 +2444,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>16</v>
       </c>
@@ -2461,7 +2473,7 @@
         <v>3636</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>16</v>
       </c>
@@ -2490,7 +2502,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>16</v>
       </c>
@@ -2519,7 +2531,7 @@
         <v>3852</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>14</v>
       </c>
@@ -2548,7 +2560,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>14</v>
       </c>
@@ -2577,7 +2589,7 @@
         <v>2610</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>14</v>
       </c>
@@ -2606,7 +2618,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>14</v>
       </c>
@@ -2635,7 +2647,7 @@
         <v>2622</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>14</v>
       </c>
@@ -2664,7 +2676,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>14</v>
       </c>
@@ -2693,7 +2705,7 @@
         <v>3288</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>14</v>
       </c>
@@ -2722,7 +2734,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>14</v>
       </c>
@@ -2751,7 +2763,7 @@
         <v>3390</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>14</v>
       </c>
@@ -2780,7 +2792,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>14</v>
       </c>
@@ -2809,7 +2821,7 @@
         <v>3510</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>14</v>
       </c>
@@ -2838,7 +2850,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>14</v>
       </c>
@@ -2867,7 +2879,7 @@
         <v>3738</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>20</v>
       </c>
@@ -2896,7 +2908,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>20</v>
       </c>
@@ -2925,7 +2937,7 @@
         <v>2514</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>15</v>
       </c>
@@ -2954,7 +2966,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>15</v>
       </c>
@@ -2983,7 +2995,7 @@
         <v>2502</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>15</v>
       </c>
@@ -3012,7 +3024,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>15</v>
       </c>
@@ -3041,7 +3053,7 @@
         <v>2838</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>15</v>
       </c>
@@ -3070,7 +3082,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>15</v>
       </c>
@@ -3099,7 +3111,7 @@
         <v>3288</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>13</v>
       </c>
@@ -3128,7 +3140,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>13</v>
       </c>
@@ -3157,7 +3169,7 @@
         <v>2838</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>18</v>
       </c>
@@ -3186,7 +3198,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>18</v>
       </c>
@@ -3215,7 +3227,7 @@
         <v>2604</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>12</v>
       </c>
@@ -3244,7 +3256,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>12</v>
       </c>
@@ -3279,24 +3291,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I69"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="8" width="12" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="5.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3325,7 +3337,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -3354,7 +3366,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -3383,7 +3395,7 @@
         <v>2616</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -3412,7 +3424,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
@@ -3441,7 +3453,7 @@
         <v>2742</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -3470,7 +3482,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -3499,7 +3511,7 @@
         <v>3402</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>10</v>
       </c>
@@ -3528,7 +3540,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>10</v>
       </c>
@@ -3557,7 +3569,7 @@
         <v>2508</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>10</v>
       </c>
@@ -3586,7 +3598,7 @@
         <v>870</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>10</v>
       </c>
@@ -3615,7 +3627,7 @@
         <v>2844</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -3644,7 +3656,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>10</v>
       </c>
@@ -3673,7 +3685,7 @@
         <v>3288</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>17</v>
       </c>
@@ -3702,7 +3714,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>17</v>
       </c>
@@ -3731,7 +3743,7 @@
         <v>2952</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>17</v>
       </c>
@@ -3760,7 +3772,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>17</v>
       </c>
@@ -3789,7 +3801,7 @@
         <v>3408</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>19</v>
       </c>
@@ -3818,7 +3830,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>19</v>
       </c>
@@ -3847,7 +3859,7 @@
         <v>2742</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>19</v>
       </c>
@@ -3876,7 +3888,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>19</v>
       </c>
@@ -3905,7 +3917,7 @@
         <v>3420</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>16</v>
       </c>
@@ -3934,7 +3946,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>16</v>
       </c>
@@ -3963,7 +3975,7 @@
         <v>2724</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>16</v>
       </c>
@@ -3992,7 +4004,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>16</v>
       </c>
@@ -4021,7 +4033,7 @@
         <v>2748</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>16</v>
       </c>
@@ -4050,7 +4062,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>16</v>
       </c>
@@ -4079,7 +4091,7 @@
         <v>3504</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>14</v>
       </c>
@@ -4108,7 +4120,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>14</v>
       </c>
@@ -4137,7 +4149,7 @@
         <v>2610</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>14</v>
       </c>
@@ -4166,7 +4178,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>14</v>
       </c>
@@ -4195,7 +4207,7 @@
         <v>2622</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>20</v>
       </c>
@@ -4224,7 +4236,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>20</v>
       </c>
@@ -4253,7 +4265,7 @@
         <v>2514</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>15</v>
       </c>
@@ -4282,7 +4294,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>15</v>
       </c>
@@ -4317,27 +4329,27 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:P45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="8" width="12" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.5" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4366,7 +4378,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -4404,7 +4416,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -4445,7 +4457,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
@@ -4474,7 +4486,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
@@ -4503,7 +4515,7 @@
         <v>3864</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -4532,7 +4544,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
@@ -4561,7 +4573,7 @@
         <v>3978</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -4590,7 +4602,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
@@ -4619,7 +4631,7 @@
         <v>3978</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>18</v>
       </c>
@@ -4648,7 +4660,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>18</v>
       </c>
@@ -4677,7 +4689,7 @@
         <v>2604</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>12</v>
       </c>
@@ -4706,7 +4718,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>12</v>
       </c>
@@ -4735,7 +4747,7 @@
         <v>2604</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>15</v>
       </c>
@@ -4764,7 +4776,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>15</v>
       </c>
@@ -4793,7 +4805,7 @@
         <v>3288</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>14</v>
       </c>
@@ -4822,7 +4834,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>14</v>
       </c>
@@ -4851,7 +4863,7 @@
         <v>3288</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>15</v>
       </c>
@@ -4880,7 +4892,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>15</v>
       </c>
@@ -4909,7 +4921,7 @@
         <v>2838</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>13</v>
       </c>
@@ -4938,7 +4950,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>13</v>
       </c>
@@ -4967,7 +4979,7 @@
         <v>2838</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>16</v>
       </c>
@@ -4996,7 +5008,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>16</v>
       </c>
@@ -5025,7 +5037,7 @@
         <v>3738</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>14</v>
       </c>
@@ -5054,7 +5066,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>14</v>
       </c>
@@ -5083,7 +5095,7 @@
         <v>3738</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>14</v>
       </c>
@@ -5112,7 +5124,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>14</v>
       </c>
@@ -5141,7 +5153,7 @@
         <v>3510</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>11</v>
       </c>
@@ -5170,7 +5182,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>11</v>
       </c>
@@ -5199,7 +5211,7 @@
         <v>3510</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>14</v>
       </c>
@@ -5228,7 +5240,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>14</v>
       </c>
@@ -5257,7 +5269,7 @@
         <v>3390</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>10</v>
       </c>
@@ -5286,7 +5298,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>10</v>
       </c>
@@ -5315,7 +5327,7 @@
         <v>3390</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>11</v>
       </c>
@@ -5344,7 +5356,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>11</v>
       </c>
@@ -5373,7 +5385,7 @@
         <v>3852</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
         <v>16</v>
       </c>
@@ -5402,7 +5414,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
         <v>16</v>
       </c>
@@ -5431,7 +5443,7 @@
         <v>3852</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
         <v>16</v>
       </c>
@@ -5460,7 +5472,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
         <v>16</v>
       </c>
@@ -5489,7 +5501,7 @@
         <v>3636</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>10</v>
       </c>
@@ -5518,7 +5530,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>10</v>
       </c>
@@ -5547,7 +5559,7 @@
         <v>3636</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>11</v>
       </c>
@@ -5576,7 +5588,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>11</v>
       </c>
@@ -5605,7 +5617,7 @@
         <v>3738</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>10</v>
       </c>
@@ -5634,7 +5646,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>10</v>
       </c>

</xml_diff>